<commit_message>
fixed typo for Kimpe
</commit_message>
<xml_diff>
--- a/raw/xlsx/numerals-kemp1234-1.xlsx
+++ b/raw/xlsx/numerals-kemp1234-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bibiko/Documents/Developments/shh_git/numeralbank/numerals/raw/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9C7714-A994-7643-A2AF-AC79B4005F71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68C5A89-9B59-5B44-A22A-F34D2CE91D0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="520" yWindow="520" windowWidth="25020" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t>基姆佩语</t>
   </si>
   <si>
-    <t>kimpe.htm</t>
-  </si>
-  <si>
     <t>CD</t>
   </si>
   <si>
@@ -252,6 +249,9 @@
   </si>
   <si>
     <t>Mai-Ndombe Province, Mushie Territory</t>
+  </si>
+  <si>
+    <t>Kimpe.htm</t>
   </si>
 </sst>
 </file>
@@ -701,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="3"/>
@@ -712,7 +712,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>21</v>
@@ -725,7 +725,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>21</v>
@@ -738,7 +738,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -749,7 +749,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>21</v>
@@ -762,7 +762,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>21</v>
@@ -775,7 +775,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>21</v>
@@ -788,7 +788,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
@@ -801,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>21</v>
@@ -814,7 +814,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -825,7 +825,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -836,7 +836,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -847,7 +847,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -858,7 +858,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -869,7 +869,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="3"/>
@@ -880,7 +880,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="7"/>
@@ -891,7 +891,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="3"/>
@@ -901,7 +901,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="7"/>
@@ -911,7 +911,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="8"/>
     </row>
@@ -920,7 +920,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="7"/>
     </row>
@@ -929,7 +929,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -937,7 +937,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -945,7 +945,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -953,7 +953,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -961,7 +961,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -969,7 +969,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -977,7 +977,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -985,7 +985,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -993,7 +993,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1001,7 +1001,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1009,7 +1009,7 @@
         <v>40</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1017,7 +1017,7 @@
         <v>50</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1025,7 +1025,7 @@
         <v>60</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1033,7 +1033,7 @@
         <v>70</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1041,7 +1041,7 @@
         <v>80</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1049,7 +1049,7 @@
         <v>90</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1057,7 +1057,7 @@
         <v>100</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1065,7 +1065,7 @@
         <v>200</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D39" s="7"/>
     </row>
@@ -1074,7 +1074,7 @@
         <v>400</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C40" s="7"/>
     </row>
@@ -1083,7 +1083,7 @@
         <v>800</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C41" s="7"/>
     </row>
@@ -1092,10 +1092,10 @@
         <v>1000</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D42" s="7">
         <v>1</v>
@@ -1106,7 +1106,7 @@
         <v>2000</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -1158,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1173,7 +1173,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.2">
@@ -1187,7 +1187,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1203,7 +1203,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1219,7 +1219,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1227,7 +1227,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1235,7 +1235,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1257,7 +1257,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1265,7 +1265,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1273,7 +1273,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1281,7 +1281,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>